<commit_message>
added two more plots
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="994" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="975" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -72,9 +72,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="[$$-409]#,##0.00;[RED]\-[$$-409]#,##0.00"/>
   </numFmts>
   <fonts count="10">
     <font>
@@ -100,37 +99,30 @@
       <family val="0"/>
     </font>
     <font>
-      <b val="true"/>
-      <i val="true"/>
-      <sz val="16"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <i val="true"/>
-      <u val="single"/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
+      <sz val="13"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="13"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="13"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -157,7 +149,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="24">
+  <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -181,22 +173,6 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -211,22 +187,18 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="10">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Heading 1" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading1 2" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Result 3" xfId="22" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Result2 4" xfId="23" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -374,6 +346,7 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -460,6 +433,7 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -546,6 +520,7 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -597,11 +572,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="79473157"/>
-        <c:axId val="77216751"/>
+        <c:axId val="33695147"/>
+        <c:axId val="26543839"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="79473157"/>
+        <c:axId val="33695147"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -645,7 +620,7 @@
           </c:tx>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -674,12 +649,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="77216751"/>
+        <c:crossAx val="26543839"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="77216751"/>
+        <c:axId val="26543839"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -732,6 +707,426 @@
           </c:tx>
           <c:overlay val="0"/>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="33695147"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="span"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Missed Event Percentage VS Avg Response Time (s)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2 devices</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$2:$E$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.028097</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.099073</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.19745</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.293826</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>46</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>4 devices</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ff420e"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$6:$E$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.013155</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.09666</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2313945</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.394554</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$6:$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14.75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>26.75</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>8 devices</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ffd320"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$10:$E$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.011846375</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.089242625</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.538235875</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.144154</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$10:$D$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.375</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.77125</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>17.6525</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:axId val="64684709"/>
+        <c:axId val="83455921"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="64684709"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Avg Response Time(s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
@@ -761,7 +1156,601 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="79473157"/>
+        <c:crossAx val="83455921"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="83455921"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Avg Missed Events %</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="64684709"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="span"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Missed Event Percentage VS Avg Turn Around Time(s)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2 devices</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$2:$F$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.13624</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.305058</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.474583</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.570439</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>46</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>4 devices</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ff420e"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$6:$F$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.070574</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.230552</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.443452</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.61029525</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$6:$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14.75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>26.75</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>8 devices</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ffd320"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$10:$F$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.070233125</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.247915625</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.947026125</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.543744375</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$10:$D$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.375</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.77125</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>17.6525</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:axId val="45568191"/>
+        <c:axId val="67636089"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="45568191"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Avg Turn Around Time (s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="67636089"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="67636089"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Avg Missed Event (%)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="45568191"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -809,9 +1798,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>257760</xdr:colOff>
+      <xdr:colOff>257400</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>161640</xdr:rowOff>
+      <xdr:rowOff>161280</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -820,11 +1809,71 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="517680" y="3817440"/>
+        <a:ext cx="5949720" cy="3239280"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>497880</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>39600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1380600</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>41040</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="1" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="6707880" y="3858480"/>
         <a:ext cx="5759640" cy="3239640"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>26280</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>69120</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1128240</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>70560</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="12665880" y="3888000"/>
+        <a:ext cx="5759640" cy="3239640"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -841,14 +1890,14 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J37" activeCellId="0" sqref="J37"/>
+      <selection pane="topLeft" activeCell="G52" activeCellId="0" sqref="G52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="5" min="1" style="1" width="19.4418604651163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="22.2744186046512"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="19.4418604651163"/>
+    <col collapsed="false" hidden="false" max="5" min="1" style="1" width="20.0604651162791"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="22.8883720930233"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="20.0604651162791"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1136,7 +2185,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="1" width="10.8279069767442"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="1" width="11.2"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
added more stuff to report. for some reason cant save to docx, so check odt
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="975" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="984" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -75,7 +75,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -118,16 +118,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="13"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -572,11 +562,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="33695147"/>
-        <c:axId val="26543839"/>
+        <c:axId val="39707652"/>
+        <c:axId val="70207379"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="33695147"/>
+        <c:axId val="39707652"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -649,12 +639,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="26543839"/>
+        <c:crossAx val="70207379"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="26543839"/>
+        <c:axId val="70207379"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -736,7 +726,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="33695147"/>
+        <c:crossAx val="39707652"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -856,6 +846,7 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -942,6 +933,7 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1028,6 +1020,7 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1079,11 +1072,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="64684709"/>
-        <c:axId val="83455921"/>
+        <c:axId val="66688016"/>
+        <c:axId val="67035773"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="64684709"/>
+        <c:axId val="66688016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1127,7 +1120,7 @@
           </c:tx>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1156,12 +1149,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="83455921"/>
+        <c:crossAx val="67035773"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="83455921"/>
+        <c:axId val="67035773"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1214,7 +1207,7 @@
           </c:tx>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1243,7 +1236,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="64684709"/>
+        <c:crossAx val="66688016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1363,6 +1356,7 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1449,6 +1443,7 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1535,6 +1530,7 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1586,11 +1582,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="45568191"/>
-        <c:axId val="67636089"/>
+        <c:axId val="60278779"/>
+        <c:axId val="62701743"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="45568191"/>
+        <c:axId val="60278779"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1634,7 +1630,7 @@
           </c:tx>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1663,12 +1659,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="67636089"/>
+        <c:crossAx val="62701743"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="67636089"/>
+        <c:axId val="62701743"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1721,7 +1717,7 @@
           </c:tx>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1750,7 +1746,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="45568191"/>
+        <c:crossAx val="60278779"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1798,9 +1794,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>257400</xdr:colOff>
+      <xdr:colOff>257040</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>161280</xdr:rowOff>
+      <xdr:rowOff>160920</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1809,7 +1805,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="517680" y="3817440"/>
-        <a:ext cx="5949720" cy="3239280"/>
+        <a:ext cx="6102000" cy="3238920"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1828,9 +1824,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1380600</xdr:colOff>
+      <xdr:colOff>1380240</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>41040</xdr:rowOff>
+      <xdr:rowOff>40680</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1838,8 +1834,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="6707880" y="3858480"/>
-        <a:ext cx="5759640" cy="3239640"/>
+        <a:off x="6860520" y="3858480"/>
+        <a:ext cx="5882760" cy="3239280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1858,9 +1854,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>1128240</xdr:colOff>
+      <xdr:colOff>1127880</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>70560</xdr:rowOff>
+      <xdr:rowOff>70200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1868,8 +1864,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="12665880" y="3888000"/>
-        <a:ext cx="5759640" cy="3239640"/>
+        <a:off x="12980160" y="3888000"/>
+        <a:ext cx="5873400" cy="3239280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1889,15 +1885,15 @@
   </sheetPr>
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G52" activeCellId="0" sqref="G52"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L46" activeCellId="0" sqref="L46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="5" min="1" style="1" width="20.0604651162791"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="22.8883720930233"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="20.0604651162791"/>
+    <col collapsed="false" hidden="false" max="5" min="1" style="1" width="20.553488372093"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="23.506976744186"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="20.553488372093"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2185,7 +2181,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="1" width="11.2"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="1" width="11.5674418604651"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>